<commit_message>
Updated stats through Game 2
Includes Game 1 and Game 2
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -271,20 +271,25 @@
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="3">
-        <v>4.0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>4.0</v>
-      </c>
-      <c r="D2" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="E2" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="F2" s="3">
-        <v>2.0</v>
+      <c r="B2" s="3" t="str">
+        <f t="shared" ref="B2:C2" si="1">4+4</f>
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="str">
+        <f t="shared" ref="D2:E2" si="2">3+3</f>
+        <v>6</v>
+      </c>
+      <c r="E2" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="str">
+        <f>2+4</f>
+        <v>6</v>
       </c>
       <c r="G2" s="3">
         <v>2.0</v>
@@ -292,8 +297,9 @@
       <c r="H2" s="3">
         <v>0.0</v>
       </c>
-      <c r="I2" s="3">
-        <v>0.0</v>
+      <c r="I2" s="3" t="str">
+        <f>0+2</f>
+        <v>2</v>
       </c>
       <c r="J2" s="3">
         <v>0.0</v>
@@ -303,43 +309,47 @@
       </c>
       <c r="L2" s="4"/>
       <c r="M2" s="5" t="str">
-        <f t="shared" ref="M2:M16" si="1">IF(C2,D2/C2,)</f>
+        <f t="shared" ref="M2:M16" si="4">IF(C2,D2/C2,)</f>
         <v>0.750</v>
       </c>
       <c r="N2" s="5" t="str">
-        <f t="shared" ref="N2:N16" si="2">IF(C2,((D2-G2-H2-I2)+(2*G2)+(3*H2)+(4*I2))/C2,)</f>
-        <v>1.250</v>
+        <f t="shared" ref="N2:N16" si="5">IF(C2,((D2-G2-H2-I2)+(2*G2)+(3*H2)+(4*I2))/C2,)</f>
+        <v>1.750</v>
       </c>
       <c r="O2" s="5" t="str">
-        <f t="shared" ref="O2:O17" si="3">IF(B2,(D2+J2)/(C2+J2),)</f>
+        <f t="shared" ref="O2:O17" si="6">IF(B2,(D2+J2)/(C2+J2),)</f>
         <v>0.750</v>
       </c>
       <c r="P2" s="5" t="str">
-        <f t="shared" ref="P2:P17" si="4">IF(N2,N2+O2,)</f>
-        <v>2.000</v>
+        <f t="shared" ref="P2:P17" si="7">IF(N2,N2+O2,)</f>
+        <v>2.500</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="3">
-        <v>4.0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>4.0</v>
-      </c>
-      <c r="D3" s="3">
-        <v>3.0</v>
+      <c r="B3" s="3" t="str">
+        <f t="shared" ref="B3:C3" si="3">4+3</f>
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="str">
+        <f>3+3</f>
+        <v>6</v>
       </c>
       <c r="E3" s="3">
         <v>2.0</v>
       </c>
-      <c r="F3" s="3">
-        <v>3.0</v>
+      <c r="F3" s="3" t="str">
+        <f>3+1</f>
+        <v>4</v>
       </c>
       <c r="G3" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H3" s="3">
         <v>0.0</v>
@@ -355,49 +365,53 @@
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>0.750</v>
+        <f t="shared" si="4"/>
+        <v>0.857</v>
       </c>
       <c r="N3" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>0.750</v>
+        <f t="shared" si="5"/>
+        <v>1.000</v>
       </c>
       <c r="O3" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>0.750</v>
+        <f t="shared" si="6"/>
+        <v>0.857</v>
       </c>
       <c r="P3" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>1.500</v>
+        <f t="shared" si="7"/>
+        <v>1.857</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="3">
-        <v>4.0</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="B4" s="3" t="str">
+        <f>4+4</f>
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="str">
+        <f t="shared" ref="C4:D4" si="8">4+2</f>
+        <v>6</v>
+      </c>
+      <c r="D4" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="E4" s="3" t="str">
+        <f>3+3</f>
+        <v>6</v>
+      </c>
+      <c r="F4" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="G4" s="3">
         <v>2.0</v>
       </c>
-      <c r="D4" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0.0</v>
-      </c>
       <c r="H4" s="3">
         <v>0.0</v>
       </c>
       <c r="I4" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J4" s="3">
         <v>2.0</v>
@@ -407,20 +421,20 @@
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.000</v>
       </c>
       <c r="N4" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
+        <v>1.833</v>
+      </c>
+      <c r="O4" s="5" t="str">
+        <f t="shared" si="6"/>
         <v>1.000</v>
       </c>
-      <c r="O4" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>1.000</v>
-      </c>
       <c r="P4" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>2.000</v>
+        <f t="shared" si="7"/>
+        <v>2.833</v>
       </c>
     </row>
     <row r="5">
@@ -459,19 +473,19 @@
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.750</v>
       </c>
       <c r="N5" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2.250</v>
       </c>
       <c r="O5" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.750</v>
       </c>
       <c r="P5" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>3.000</v>
       </c>
     </row>
@@ -479,20 +493,25 @@
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="3">
-        <v>4.0</v>
-      </c>
-      <c r="C6" s="3">
-        <v>4.0</v>
-      </c>
-      <c r="D6" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="F6" s="3">
-        <v>1.0</v>
+      <c r="B6" s="3" t="str">
+        <f t="shared" ref="B6:C6" si="9">4+4</f>
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="D6" s="3" t="str">
+        <f>2+2</f>
+        <v>4</v>
+      </c>
+      <c r="E6" s="3" t="str">
+        <f>1+2</f>
+        <v>3</v>
+      </c>
+      <c r="F6" s="3" t="str">
+        <f t="shared" ref="F6:F7" si="11">1+1</f>
+        <v>2</v>
       </c>
       <c r="G6" s="3">
         <v>0.0</v>
@@ -511,19 +530,19 @@
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.500</v>
       </c>
       <c r="N6" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.500</v>
       </c>
       <c r="O6" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.500</v>
       </c>
       <c r="P6" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.000</v>
       </c>
     </row>
@@ -531,23 +550,27 @@
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="C7" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="D7" s="3">
+      <c r="B7" s="3" t="str">
+        <f t="shared" ref="B7:C7" si="10">3+3</f>
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="str">
+        <f>1+1</f>
+        <v>2</v>
+      </c>
+      <c r="E7" s="3">
         <v>1.0</v>
       </c>
-      <c r="E7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F7" s="3">
+      <c r="F7" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="G7" s="3">
         <v>1.0</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0.0</v>
       </c>
       <c r="H7" s="3">
         <v>0.0</v>
@@ -563,40 +586,45 @@
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.333</v>
       </c>
       <c r="N7" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
+        <v>0.500</v>
+      </c>
+      <c r="O7" s="5" t="str">
+        <f t="shared" si="6"/>
         <v>0.333</v>
       </c>
-      <c r="O7" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>0.333</v>
-      </c>
       <c r="P7" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>0.667</v>
+        <f t="shared" si="7"/>
+        <v>0.833</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="C8" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0.0</v>
+      <c r="B8" s="3" t="str">
+        <f t="shared" ref="B8:C8" si="12">3+3</f>
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="str">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="D8" s="3" t="str">
+        <f>2+2</f>
+        <v>4</v>
+      </c>
+      <c r="E8" s="3" t="str">
+        <f>2+1</f>
+        <v>3</v>
+      </c>
+      <c r="F8" s="3" t="str">
+        <f>0+2</f>
+        <v>2</v>
       </c>
       <c r="G8" s="3">
         <v>0.0</v>
@@ -615,19 +643,19 @@
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.667</v>
       </c>
       <c r="N8" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.667</v>
       </c>
       <c r="O8" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.667</v>
       </c>
       <c r="P8" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.333</v>
       </c>
     </row>
@@ -635,17 +663,21 @@
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="C9" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1.0</v>
+      <c r="B9" s="3" t="str">
+        <f t="shared" ref="B9:C9" si="13">3+3</f>
+        <v>6</v>
+      </c>
+      <c r="C9" s="3" t="str">
+        <f t="shared" si="13"/>
+        <v>6</v>
+      </c>
+      <c r="D9" s="3" t="str">
+        <f>1+2</f>
+        <v>3</v>
+      </c>
+      <c r="E9" s="3" t="str">
+        <f>1+1</f>
+        <v>2</v>
       </c>
       <c r="F9" s="3">
         <v>0.0</v>
@@ -667,46 +699,50 @@
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>0.333</v>
+        <f t="shared" si="4"/>
+        <v>0.500</v>
       </c>
       <c r="N9" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>0.333</v>
+        <f t="shared" si="5"/>
+        <v>0.500</v>
       </c>
       <c r="O9" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>0.333</v>
+        <f t="shared" si="6"/>
+        <v>0.500</v>
       </c>
       <c r="P9" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>0.667</v>
+        <f t="shared" si="7"/>
+        <v>1.000</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="C10" s="3">
-        <v>3.0</v>
+      <c r="B10" s="3" t="str">
+        <f t="shared" ref="B10:C10" si="14">3+3</f>
+        <v>6</v>
+      </c>
+      <c r="C10" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>6</v>
       </c>
       <c r="D10" s="3">
         <v>2.0</v>
       </c>
-      <c r="E10" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="F10" s="3">
-        <v>2.0</v>
+      <c r="E10" s="3" t="str">
+        <f t="shared" ref="E10:F10" si="15">2+1</f>
+        <v>3</v>
+      </c>
+      <c r="F10" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>3</v>
       </c>
       <c r="G10" s="3">
         <v>0.0</v>
       </c>
       <c r="H10" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I10" s="3">
         <v>0.0</v>
@@ -719,46 +755,47 @@
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
+        <v>0.333</v>
+      </c>
+      <c r="N10" s="5" t="str">
+        <f t="shared" si="5"/>
         <v>0.667</v>
       </c>
-      <c r="N10" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>0.667</v>
-      </c>
       <c r="O10" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>0.667</v>
+        <f t="shared" si="6"/>
+        <v>0.333</v>
       </c>
       <c r="P10" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>1.333</v>
+        <f t="shared" si="7"/>
+        <v>1.000</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="3">
-        <v>0.0</v>
+      <c r="B11" s="3" t="str">
+        <f>4</f>
+        <v>4</v>
       </c>
       <c r="C11" s="3">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="D11" s="3">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="E11" s="3">
         <v>0.0</v>
       </c>
       <c r="F11" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G11" s="3">
         <v>0.0</v>
       </c>
       <c r="H11" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I11" s="3">
         <v>0.0</v>
@@ -771,20 +808,20 @@
       </c>
       <c r="L11" s="4"/>
       <c r="M11" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <f t="shared" si="4"/>
+        <v>0.750</v>
       </c>
       <c r="N11" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+        <f t="shared" si="5"/>
+        <v>1.250</v>
       </c>
       <c r="O11" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <f t="shared" si="6"/>
+        <v>0.750</v>
       </c>
       <c r="P11" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" si="7"/>
+        <v>2.000</v>
       </c>
     </row>
     <row r="12">
@@ -823,19 +860,19 @@
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N12" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O12" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P12" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -875,19 +912,19 @@
       </c>
       <c r="L13" s="4"/>
       <c r="M13" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N13" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O13" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P13" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -896,16 +933,16 @@
         <v>27</v>
       </c>
       <c r="B14" s="3">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="C14" s="3">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="D14" s="3">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="E14" s="3">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="F14" s="3">
         <v>0.0</v>
@@ -927,20 +964,20 @@
       </c>
       <c r="L14" s="4"/>
       <c r="M14" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <f t="shared" si="4"/>
+        <v>0.500</v>
       </c>
       <c r="N14" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+        <f t="shared" si="5"/>
+        <v>0.500</v>
       </c>
       <c r="O14" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <f t="shared" si="6"/>
+        <v>0.500</v>
       </c>
       <c r="P14" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" si="7"/>
+        <v>1.000</v>
       </c>
     </row>
     <row r="15">
@@ -979,19 +1016,19 @@
       </c>
       <c r="L15" s="4"/>
       <c r="M15" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.000</v>
       </c>
       <c r="N15" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.667</v>
       </c>
       <c r="O15" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.000</v>
       </c>
       <c r="P15" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>2.667</v>
       </c>
     </row>
@@ -1031,19 +1068,19 @@
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.333</v>
       </c>
       <c r="N16" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.333</v>
       </c>
       <c r="O16" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.500</v>
       </c>
       <c r="P16" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.833</v>
       </c>
     </row>
@@ -1052,61 +1089,61 @@
         <v>30</v>
       </c>
       <c r="B17" s="1" t="str">
-        <f t="shared" ref="B17:K17" si="5">sum(B2:B16)</f>
-        <v>39</v>
+        <f t="shared" ref="B17:K17" si="16">sum(B2:B16)</f>
+        <v>74</v>
       </c>
       <c r="C17" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>36</v>
+        <f t="shared" si="16"/>
+        <v>71</v>
       </c>
       <c r="D17" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>23</v>
+        <f t="shared" si="16"/>
+        <v>45</v>
       </c>
       <c r="E17" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>18</v>
+        <f t="shared" si="16"/>
+        <v>32</v>
       </c>
       <c r="F17" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>18</v>
+        <f t="shared" si="16"/>
+        <v>32</v>
       </c>
       <c r="G17" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f t="shared" si="16"/>
+        <v>8</v>
       </c>
       <c r="H17" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="16"/>
+        <v>5</v>
+      </c>
+      <c r="I17" s="1" t="str">
+        <f t="shared" si="16"/>
         <v>3</v>
       </c>
-      <c r="I17" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="J17" s="1" t="str">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="K17" s="1" t="str">
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="J17" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="K17" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L17" s="4"/>
+      <c r="L17" s="3"/>
       <c r="M17" s="6" t="str">
         <f>D17/C17</f>
-        <v>0.639</v>
+        <v>0.634</v>
       </c>
       <c r="N17" s="6" t="str">
         <f>((D17-G17-H17-I17)+(2*G17)+(3*H17)+(4*I17))/C17</f>
-        <v>0.917</v>
+        <v>1.014</v>
       </c>
       <c r="O17" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v>0.667</v>
+        <f t="shared" si="6"/>
+        <v>0.649</v>
       </c>
       <c r="P17" s="6" t="str">
-        <f t="shared" si="4"/>
-        <v>1.583</v>
+        <f t="shared" si="7"/>
+        <v>1.663</v>
       </c>
     </row>
     <row r="21">

</xml_diff>